<commit_message>
Notes from Senate hearing on S.881 durin the 97th Congress
</commit_message>
<xml_diff>
--- a/FinalProject/LiteratureReview/Townes_POLS6310_FinalProject_Notes_v00.xlsx
+++ b/FinalProject/LiteratureReview/Townes_POLS6310_FinalProject_Notes_v00.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="71">
   <si>
     <t>Full Citation</t>
   </si>
@@ -160,32 +160,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The Small Business Innovation Research Act of 1981</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Hearings before the Subcommittee on Innovation and Technology of the Senate Committee on Small Business, 97th Cong. 1-4 (1981) (Statement of Senator Warren Rudman).</t>
-    </r>
-  </si>
-  <si>
-    <t>The Small Business Innovation Research Act of 1981: Hearings before the Subcommittee on Innovation and Technology of the Senate Committee on Small Business, 97th Cong. 5 (1981) (Statement of Senator Paul Tsongas).</t>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Statement of Senator Paul Tsongas in </t>
     </r>
     <r>
@@ -211,8 +185,32 @@
     </r>
   </si>
   <si>
+    <t>The Federal government has been failing to leverage innovation from small businesses.</t>
+  </si>
+  <si>
+    <t>Statement of Senator Paul Tsongas in The Small Business Innovation Research Act of 1981 (1981).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entrepreneurs who launched small technology-based ventures that grew into companies that employ more than 1,000 people rescued Massachusetts from economic stagnation. </t>
+  </si>
+  <si>
+    <t>Small firms are faster, more productive innovators because they are led by creative, risk-taking entrepreneurs whereas as large firms are led by prudent, efficiency-minded, risk-adverse corporate executives.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A set-aside program is needed because the way Federal research and development funding is awarded strongly favors large, nationally known companies.  Contract officers are tasked with awarding and monitoring  a certain amount of contracts make more efficient use of their time by awarding larger contracts to a smaller number of recipients.  Only large businesses have the infrastructure and wherewithal to employ and manage such large funding awards.  Favoring large businesses also minimizes the risk of mismanagement by the recipient which could hurt the contract officer professionally. </t>
+  </si>
+  <si>
+    <t>8-9</t>
+  </si>
+  <si>
+    <t>The goal is to yield the greatest amount of benefit from every federal dollar spent.</t>
+  </si>
+  <si>
+    <t>Senator Edward M. Kennedy was a long-time supporter of the approach outlined in the legislation.</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Testimony of [Name] in </t>
+      <t xml:space="preserve">Statement of Senator Edward Kennedy in </t>
     </r>
     <r>
       <rPr>
@@ -237,28 +235,117 @@
     </r>
   </si>
   <si>
-    <t>The Federal government has been failing to leverage innovation from small businesses.</t>
-  </si>
-  <si>
-    <t>Statement of Senator Paul Tsongas in The Small Business Innovation Research Act of 1981 (1981).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entrepreneurs who launched small technology-based ventures that grew into companies that employ more than 1,000 people rescued Massachusetts from economic stagnation. </t>
-  </si>
-  <si>
-    <t>Small firms are faster, more productive innovators because they are led by creative, risk-taking entrepreneurs whereas as large firms are led by prudent, efficiency-minded, risk-adverse corporate executives.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A set-aside program is needed because the way Federal research and development funding is awarded strongly favors large, nationally known companies.  Contract officers are tasked with awarding and monitoring  a certain amount of contracts make more efficient use of their time by awarding larger contracts to a smaller number of recipients.  Only large businesses have the infrastructure and wherewithal to employ and manage such large funding awards.  Favoring large businesses also minimizes the risk of mismanagement by the recipient which could hurt the contract officer professionally. </t>
-  </si>
-  <si>
-    <t>8-9</t>
-  </si>
-  <si>
-    <t>The goal is to yield the greatest amount of benefit from every federal dollar spent.</t>
-  </si>
-  <si>
-    <t>Senator Edward M. Kennedy was a long-time supporter of the approach outlined in the legislation.</t>
+    <t>Statement of Senator Edward Kennedy in The Small Business Innovation Research Act of 1981 (1981).</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>New innovation by businesses is necessary for the economic recovery of the nation, which is currently suffering from high inflation, unemployment, and interest rates.</t>
+  </si>
+  <si>
+    <t>The Small Business Innovation Research Act was introduced by Senators Rudman, Tsongas, and Kennedy.</t>
+  </si>
+  <si>
+    <t>Senator Kennedy introduced the legislation that created the three-phase small business innovation research program in the National Science Foundation, which is the template for the currently proposed program.</t>
+  </si>
+  <si>
+    <t>Testimony of [Name] in The Small Business Innovation Research Act of 1981 (1981).</t>
+  </si>
+  <si>
+    <t>The Small Business Innovation Research Act of 1981: Hearings before the Subcommittee on Innovation and Technology of the Senate Committee on Small Business, 97th Cong. 11 (1981) (testimony of Peter T. Webster).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Testimony of Peter T. Webster in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Small Business Innovation Research Act of 1981</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (1981).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Small Business Innovation Research Act of 1981</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Hearings before the Subcommittee on Innovation and Technology of the Senate Committee on Small Business, 97th Cong. 1-4 (1981) (statement of Senator Warren Rudman).</t>
+    </r>
+  </si>
+  <si>
+    <t>The Small Business Innovation Research Act of 1981: Hearings before the Subcommittee on Innovation and Technology of the Senate Committee on Small Business, 97th Cong. 5-9 (1981) (statement of Senator Paul Tsongas).</t>
+  </si>
+  <si>
+    <t>The Small Business Innovation Research Act of 1981: Hearings before the Subcommittee on Innovation and Technology of the Senate Committee on Small Business, 97th Cong. 10 (1981) (statement of Senator Edward M. Kennedy).</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Testimony of Peter T. Webster in The Small Business Innovation Research Act of 1981 (1981).</t>
+  </si>
+  <si>
+    <t>Small companies produce up to 24 times more innovations per research and development dollar than big companies.
+COMMENT: What is defined as an innovation?  What is defined as a small business?</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>Equity</t>
+  </si>
+  <si>
+    <t>Welfare</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Small businesses want equal access, not preferential treatment.</t>
+  </si>
+  <si>
+    <t>Large businesses use innovation as a means to block competition from the market. They substitute capital for jobs.  Innovation by small businesses create new markets and jobs.</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>There are groups that want to limit the role of Federal government in supporting small business research and development.</t>
+  </si>
+  <si>
+    <t>One of the objections to the bill is that it discriminates in favor of small businesses and that it provides small businesses with an unfair advantage over the rest of the research and development community.  The advisory committee on industrial innovation argues that "Government policies and regulations that treat large and small firms equally are ini fact discriminatory against small firms."</t>
   </si>
 </sst>
 </file>
@@ -649,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,7 +775,7 @@
     </row>
     <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>20</v>
@@ -696,26 +783,34 @@
     </row>
     <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>41</v>
+      <c r="B8" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -732,13 +827,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U20"/>
+  <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,9 +841,7 @@
     <col min="1" max="1" width="50.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="6" customWidth="1"/>
     <col min="3" max="3" width="75.7109375" style="1" customWidth="1"/>
-    <col min="4" max="9" width="10.7109375" style="5" customWidth="1"/>
-    <col min="10" max="12" width="10.7109375" style="1" customWidth="1"/>
-    <col min="13" max="20" width="10.7109375" style="5" customWidth="1"/>
+    <col min="4" max="20" width="10.7109375" style="5" customWidth="1"/>
     <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -780,9 +873,15 @@
       <c r="I1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
+      <c r="J1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
@@ -893,6 +992,9 @@
       <c r="H8" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="L8" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -921,6 +1023,9 @@
       <c r="F10" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="K10" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -935,6 +1040,9 @@
       <c r="F11" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="J11" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -983,13 +1091,13 @@
     </row>
     <row r="15" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>10</v>
@@ -1000,13 +1108,13 @@
     </row>
     <row r="16" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>10</v>
@@ -1015,15 +1123,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>10</v>
@@ -1032,15 +1140,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>10</v>
@@ -1051,32 +1159,156 @@
       <c r="H18" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="J18" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="C21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="B22" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Notes from lecture on February 18, 2019
</commit_message>
<xml_diff>
--- a/FinalProject/LiteratureReview/Townes_POLS6310_FinalProject_Notes_v00.xlsx
+++ b/FinalProject/LiteratureReview/Townes_POLS6310_FinalProject_Notes_v00.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="88">
   <si>
     <t>Full Citation</t>
   </si>
@@ -346,6 +346,57 @@
   </si>
   <si>
     <t>One of the objections to the bill is that it discriminates in favor of small businesses and that it provides small businesses with an unfair advantage over the rest of the research and development community.  The advisory committee on industrial innovation argues that "Government policies and regulations that treat large and small firms equally are ini fact discriminatory against small firms."</t>
+  </si>
+  <si>
+    <t>The Small Business Innovation Research Act of 1981: Hearings before the Subcommittee on Innovation and Technology of the Senate Committee on Small Business, 97th Cong. [pp] (1981) (testimony of Robert E. Patterson).</t>
+  </si>
+  <si>
+    <t>Testimony of Robert E. Patterson in The Small Business Innovation Research Act of 1981 (1981).</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Between 1960 and 1975, Massachusetts lost one-fifth (over 120,000 jobs) of its manufacturing jobs.</t>
+  </si>
+  <si>
+    <t>In 1975, the unemployment rate in Massachusetts was 50 percent more than the National average.</t>
+  </si>
+  <si>
+    <t>Massachusetts Industrial Finance Agency (MIFA) was a supporter of the legislation.</t>
+  </si>
+  <si>
+    <t>MIFA focuses its programs on small innovative companies which it believes are more efficient and more productive.  More than half have annual revenues of less than $5 million and 75 percent have annual revenues less than $25 million.</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Seed-stage funding to take an idea from conceptual and theoretical stage to operational prototype is the most difficult to obtain.  MIFA is not equipped to make those kinds of investments; it's an employment-generating program focused of manufacturing operations.</t>
+  </si>
+  <si>
+    <t>The Small Business Innovation Research Act of 1981: Hearings before the Subcommittee on Innovation and Technology of the Senate Committee on Small Business, 97th Cong. [pp] (1981) (testimony of John Tillinghast).</t>
+  </si>
+  <si>
+    <t>Testimony of John Tillinghast in The Small Business Innovation Research Act of 1981 (1981).</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>Small firms are more innovative than large firms because they have less structure to impede them. COMMENT: Hypothesis; unsupported ascertion.</t>
+  </si>
+  <si>
+    <t>Expanded technological innovation is essential for the success of the Nation.  In recent years the number of new technological innovations has been declining while it has been increasing in other countries.  COMMENT: Hypothesis; unsupport ascertion.</t>
+  </si>
+  <si>
+    <t>Symbolism</t>
+  </si>
+  <si>
+    <t>Other countries are devoting enormous resources to create small technology companies that have significant growth potential. COMMENT: Unsupported ascertion</t>
   </si>
 </sst>
 </file>
@@ -736,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,11 +856,27 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>53</v>
       </c>
     </row>
@@ -827,13 +894,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U28"/>
+  <dimension ref="A1:U36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A29" sqref="A29"/>
+      <selection pane="bottomRight" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,7 +949,9 @@
       <c r="L1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="4"/>
+      <c r="M1" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
@@ -1309,6 +1378,130 @@
         <v>10</v>
       </c>
       <c r="J28" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F36" s="5" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>